<commit_message>
big modifications for elliminating Inputs
</commit_message>
<xml_diff>
--- a/inputs/PortfolioMarc.xlsx
+++ b/inputs/PortfolioMarc.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marc_\Dropbox\MLosPython\PortfolioAlgorithm\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E044889C-AAA5-40FF-9F34-295C90C7B4EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39328FB5-D6F9-4564-ABDB-3E20A603E70D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="16220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="16220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="P1" sheetId="1" r:id="rId1"/>
-    <sheet name="Resources" sheetId="2" r:id="rId2"/>
+    <sheet name="P2" sheetId="3" r:id="rId2"/>
+    <sheet name="P3" sheetId="4" r:id="rId3"/>
+    <sheet name="Resources" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="22">
   <si>
     <t>R1</t>
   </si>
@@ -585,7 +587,7 @@
   </sheetPr>
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+    <sheetView zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
       <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
@@ -740,6 +742,328 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F1BA12B-D073-4557-8694-B76E40E6671C}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.7265625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="51.453125" customWidth="1"/>
+    <col min="3" max="3" width="54" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.81640625" customWidth="1"/>
+    <col min="5" max="5" width="23.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="14" x14ac:dyDescent="0.3">
+      <c r="A2" s="10">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="7">
+        <v>0</v>
+      </c>
+      <c r="E2" s="5"/>
+      <c r="F2" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+    </row>
+    <row r="3" spans="1:8" ht="14" x14ac:dyDescent="0.3">
+      <c r="A3" s="11">
+        <v>2</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="7">
+        <v>80</v>
+      </c>
+      <c r="E3" s="6">
+        <v>1</v>
+      </c>
+      <c r="F3" s="13">
+        <v>5</v>
+      </c>
+      <c r="G3" s="8">
+        <v>1</v>
+      </c>
+      <c r="H3" s="8"/>
+    </row>
+    <row r="4" spans="1:8" ht="14" x14ac:dyDescent="0.3">
+      <c r="A4" s="11">
+        <v>3</v>
+      </c>
+      <c r="B4" s="20"/>
+      <c r="C4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="7">
+        <v>80</v>
+      </c>
+      <c r="E4" s="6">
+        <v>1</v>
+      </c>
+      <c r="F4" s="13">
+        <v>5</v>
+      </c>
+      <c r="G4" s="8">
+        <v>1</v>
+      </c>
+      <c r="H4" s="8"/>
+    </row>
+    <row r="5" spans="1:8" ht="14" x14ac:dyDescent="0.3">
+      <c r="A5" s="11">
+        <v>4</v>
+      </c>
+      <c r="B5" s="20"/>
+      <c r="C5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="7">
+        <v>80</v>
+      </c>
+      <c r="E5" s="6">
+        <v>1</v>
+      </c>
+      <c r="F5" s="13">
+        <v>5</v>
+      </c>
+      <c r="G5" s="8">
+        <v>1</v>
+      </c>
+      <c r="H5" s="8"/>
+    </row>
+    <row r="6" spans="1:8" ht="14" x14ac:dyDescent="0.3">
+      <c r="A6" s="11">
+        <v>5</v>
+      </c>
+      <c r="B6" s="20"/>
+      <c r="C6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="7">
+        <v>0</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="13"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:B6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BE063BD-F223-4E91-B9D9-6781541061CD}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.7265625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="51.453125" customWidth="1"/>
+    <col min="3" max="3" width="54" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.81640625" customWidth="1"/>
+    <col min="5" max="5" width="23.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="14" x14ac:dyDescent="0.3">
+      <c r="A2" s="10">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="7">
+        <v>0</v>
+      </c>
+      <c r="E2" s="5"/>
+      <c r="F2" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+    </row>
+    <row r="3" spans="1:8" ht="14" x14ac:dyDescent="0.3">
+      <c r="A3" s="11">
+        <v>2</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="7">
+        <v>80</v>
+      </c>
+      <c r="E3" s="6">
+        <v>1</v>
+      </c>
+      <c r="F3" s="13">
+        <v>5</v>
+      </c>
+      <c r="G3" s="8">
+        <v>1</v>
+      </c>
+      <c r="H3" s="8"/>
+    </row>
+    <row r="4" spans="1:8" ht="14" x14ac:dyDescent="0.3">
+      <c r="A4" s="11">
+        <v>3</v>
+      </c>
+      <c r="B4" s="20"/>
+      <c r="C4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="7">
+        <v>80</v>
+      </c>
+      <c r="E4" s="6">
+        <v>1</v>
+      </c>
+      <c r="F4" s="13">
+        <v>5</v>
+      </c>
+      <c r="G4" s="8">
+        <v>1</v>
+      </c>
+      <c r="H4" s="8"/>
+    </row>
+    <row r="5" spans="1:8" ht="14" x14ac:dyDescent="0.3">
+      <c r="A5" s="11">
+        <v>4</v>
+      </c>
+      <c r="B5" s="20"/>
+      <c r="C5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="7">
+        <v>80</v>
+      </c>
+      <c r="E5" s="6">
+        <v>1</v>
+      </c>
+      <c r="F5" s="13">
+        <v>5</v>
+      </c>
+      <c r="G5" s="8">
+        <v>1</v>
+      </c>
+      <c r="H5" s="8"/>
+    </row>
+    <row r="6" spans="1:8" ht="14" x14ac:dyDescent="0.3">
+      <c r="A6" s="11">
+        <v>5</v>
+      </c>
+      <c r="B6" s="20"/>
+      <c r="C6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="7">
+        <v>0</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="13"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:B6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21CB802F-0475-496E-8822-0B57475D2D84}">
   <dimension ref="A1:D3"/>
   <sheetViews>

</xml_diff>

<commit_message>
major update: external predecessors working
</commit_message>
<xml_diff>
--- a/inputs/PortfolioMarc.xlsx
+++ b/inputs/PortfolioMarc.xlsx
@@ -85,7 +85,7 @@
     <t>FINAL DESIGN REVIEW</t>
   </si>
   <si>
-    <t>P3-2</t>
+    <t>P3-5</t>
   </si>
 </sst>
 </file>
@@ -110,7 +110,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -309,7 +309,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="37">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -330,7 +330,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -413,17 +413,11 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -733,15 +727,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="36" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="37" width="51.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="37" width="54.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="36" width="12.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="36" width="23.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="38" width="23.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="31" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="32" width="51.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="32" width="54.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="33" width="12.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="33" width="23.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="34" width="23.14785714285714" customWidth="1" bestFit="1"/>
     <col min="7" max="7" style="7" width="23.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="36" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="37" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="35" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="36" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75" customFormat="1" s="9">
@@ -911,9 +905,9 @@
     <col min="4" max="4" style="33" width="12.862142857142858" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="33" width="23.14785714285714" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="34" width="23.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="35" width="23.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="36" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="37" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="7" width="23.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="35" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="36" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75" customFormat="1" s="9">
@@ -1037,7 +1031,7 @@
       </c>
       <c r="I5" s="22"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="23">
         <v>5</v>
       </c>
@@ -1081,9 +1075,9 @@
     <col min="4" max="4" style="33" width="12.862142857142858" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="33" width="23.14785714285714" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="34" width="23.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="35" width="23.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="36" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="37" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="7" width="23.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="35" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="36" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75" customFormat="1" s="9">
@@ -1207,7 +1201,7 @@
       </c>
       <c r="I5" s="22"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="23">
         <v>5</v>
       </c>

</xml_diff>